<commit_message>
mais compras na folha
</commit_message>
<xml_diff>
--- a/reports/compras.xlsx
+++ b/reports/compras.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Item</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>oled 0,91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB </t>
+  </si>
+  <si>
+    <t>header 8 pinos</t>
+  </si>
+  <si>
+    <t>header 6 pinos</t>
+  </si>
+  <si>
+    <t>conector jst</t>
+  </si>
+  <si>
+    <t>bateria</t>
+  </si>
+  <si>
+    <t>carregador da bateria</t>
+  </si>
+  <si>
+    <t>pente 40 pinos</t>
   </si>
 </sst>
 </file>
@@ -59,7 +80,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -92,7 +113,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,8 +435,8 @@
         <v>3.99</v>
       </c>
       <c r="E2" s="1">
-        <f>SUM(C2:C10)</f>
-        <v>18.900000000000002</v>
+        <f>SUM(C2:C20)</f>
+        <v>41.96</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -448,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1">
-        <v>1.04</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -474,13 +495,81 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="1"/>
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.65</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more stuff on the reports, final design for presentation on the heart module
</commit_message>
<xml_diff>
--- a/reports/compras.xlsx
+++ b/reports/compras.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Item</t>
   </si>
@@ -85,14 +85,16 @@
   </si>
   <si>
     <t>Valor</t>
+  </si>
+  <si>
+    <t>interruptor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
@@ -124,10 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +429,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D1" t="s">
@@ -450,7 +451,7 @@
       </c>
       <c r="E2" s="1">
         <f>SUM(C2:C20)</f>
-        <v>59.410000000000004</v>
+        <v>60.66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -576,7 +577,7 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>8.5</v>
       </c>
     </row>
@@ -587,7 +588,7 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>0.65</v>
       </c>
     </row>
@@ -598,7 +599,7 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>7.95</v>
       </c>
     </row>
@@ -609,8 +610,16 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="1">
         <v>8.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>